<commit_message>
Update papers and simulators
</commit_message>
<xml_diff>
--- a/simulators.xlsx
+++ b/simulators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Documents\GitHub\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E54EE1E-E0FD-44D3-8EEB-6666CF69E94C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA247D5-EDF5-4176-B5D6-08138101DDDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{4E9B9DB1-AD86-462F-ABE1-AF8EFB24C250}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="267">
   <si>
     <t>https://www.researchgate.net/post/How_can_I_implement_fog_computing_in_NetSim</t>
   </si>
@@ -845,12 +845,6 @@
     <t>https://github.com/SEI-TTG/pycloud/wiki</t>
   </si>
   <si>
-    <t>KD-Cloudlet</t>
-  </si>
-  <si>
-    <t>Software implementation19 of an in-the-field solution for establishing trusted identities in disconnected edge environments.</t>
-  </si>
-  <si>
     <t>Federation Policy</t>
   </si>
   <si>
@@ -861,6 +855,18 @@
   </si>
   <si>
     <t xml:space="preserve"> +/-</t>
+  </si>
+  <si>
+    <t>iFogStor</t>
+  </si>
+  <si>
+    <t>An IoT Data Placement Strategy for Fog Infrastructure.</t>
+  </si>
+  <si>
+    <t>pycloud</t>
+  </si>
+  <si>
+    <t>Python-based Cloudlet Server component of KD-Cloudlet, an infrastructure for VM-based cyber-foraging.</t>
   </si>
 </sst>
 </file>
@@ -1349,9 +1355,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{766B7034-B3C3-4E86-9F1C-C72AFBD67B0A}">
-  <dimension ref="A1:R56"/>
+  <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1399,7 +1407,7 @@
         <v>196</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="N1" s="20" t="s">
         <v>195</v>
@@ -1452,7 +1460,7 @@
         <v>157</v>
       </c>
       <c r="R2" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1508,7 +1516,7 @@
         <v>157</v>
       </c>
       <c r="R3" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -1538,7 +1546,7 @@
         <v>157</v>
       </c>
       <c r="R4" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -1568,7 +1576,7 @@
         <v>157</v>
       </c>
       <c r="R5" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -1598,7 +1606,7 @@
         <v>157</v>
       </c>
       <c r="R6" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -1634,7 +1642,7 @@
         <v>157</v>
       </c>
       <c r="R7" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -1670,7 +1678,7 @@
         <v>157</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="72" x14ac:dyDescent="0.3">
@@ -1700,7 +1708,7 @@
         <v>157</v>
       </c>
       <c r="R9" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -1730,7 +1738,7 @@
         <v>157</v>
       </c>
       <c r="R10" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -1776,7 +1784,7 @@
         <v>157</v>
       </c>
       <c r="R11" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -1806,7 +1814,7 @@
         <v>157</v>
       </c>
       <c r="R12" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -1836,7 +1844,7 @@
         <v>157</v>
       </c>
       <c r="R13" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -1888,7 +1896,7 @@
         <v>157</v>
       </c>
       <c r="R14" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -1918,7 +1926,7 @@
         <v>155</v>
       </c>
       <c r="R15" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -1950,7 +1958,7 @@
         <v>209</v>
       </c>
       <c r="R16" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -1980,7 +1988,7 @@
         <v>212</v>
       </c>
       <c r="R17" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -2010,7 +2018,7 @@
         <v>147</v>
       </c>
       <c r="R18" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
@@ -2040,7 +2048,7 @@
         <v>141</v>
       </c>
       <c r="R19" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -2070,7 +2078,7 @@
         <v>226</v>
       </c>
       <c r="R20" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -2100,7 +2108,7 @@
         <v>137</v>
       </c>
       <c r="R21" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -2130,7 +2138,7 @@
         <v>132</v>
       </c>
       <c r="R22" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -2162,7 +2170,7 @@
         <v>128</v>
       </c>
       <c r="R23" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -2218,7 +2226,7 @@
         <v>118</v>
       </c>
       <c r="R24" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -2266,7 +2274,7 @@
         <v>106</v>
       </c>
       <c r="R25" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="72" x14ac:dyDescent="0.3">
@@ -2302,7 +2310,7 @@
       </c>
       <c r="Q26" s="15"/>
       <c r="R26" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
@@ -2352,7 +2360,7 @@
       </c>
       <c r="Q27" s="18"/>
       <c r="R27" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -2400,7 +2408,7 @@
         <v>76</v>
       </c>
       <c r="R28" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
@@ -2436,7 +2444,7 @@
         <v>51</v>
       </c>
       <c r="R29" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -2472,7 +2480,7 @@
         <v>43</v>
       </c>
       <c r="R30" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -2508,7 +2516,7 @@
         <v>40</v>
       </c>
       <c r="R31" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
@@ -2542,16 +2550,16 @@
       </c>
       <c r="Q32" s="18"/>
       <c r="R32" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="19" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
-      <c r="D33" s="18" t="s">
+      <c r="D33" s="17" t="s">
         <v>14</v>
       </c>
       <c r="E33" s="17"/>
@@ -2564,108 +2572,100 @@
       <c r="L33" s="17"/>
       <c r="M33" s="17"/>
       <c r="N33" s="17"/>
-      <c r="O33" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="P33" s="16" t="s">
-        <v>13</v>
+      <c r="O33" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="P33" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="Q33" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="R33" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="R33" s="12" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="P34" s="13" t="s">
-        <v>10</v>
+        <v>227</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="O34" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="P34" s="5" t="s">
+        <v>230</v>
       </c>
       <c r="Q34" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="R34" s="12" t="s">
-        <v>264</v>
+        <v>228</v>
+      </c>
+      <c r="R34" s="8" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
+        <v>233</v>
+      </c>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
       <c r="D35" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
-      <c r="M35" s="17"/>
-      <c r="N35" s="17"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
       <c r="O35" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="P35" s="10" t="s">
-        <v>7</v>
+      <c r="P35" s="16" t="s">
+        <v>231</v>
       </c>
       <c r="Q35" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="R35" s="12" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+      <c r="R35" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>68</v>
+        <v>234</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>14</v>
       </c>
       <c r="O36" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="P36" s="5" t="s">
-        <v>222</v>
+      <c r="P36" s="13" t="s">
+        <v>235</v>
       </c>
       <c r="Q36" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="R36" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="R36" s="12" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
+      <c r="D37" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
       <c r="G37" s="18"/>
@@ -2676,22 +2676,22 @@
       <c r="L37" s="18"/>
       <c r="M37" s="18"/>
       <c r="N37" s="18"/>
-      <c r="O37" s="18" t="s">
-        <v>16</v>
+      <c r="O37" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="P37" s="16" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="Q37" s="15" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="R37" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="D38" s="20" t="s">
         <v>14</v>
@@ -2699,19 +2699,19 @@
       <c r="O38" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="P38" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q38" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="R38" s="8" t="s">
-        <v>263</v>
+      <c r="P38" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q38" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="R38" s="12" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="19" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
@@ -2732,18 +2732,18 @@
         <v>20</v>
       </c>
       <c r="P39" s="16" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="Q39" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="R39" s="8" t="s">
-        <v>263</v>
+        <v>240</v>
+      </c>
+      <c r="R39" s="12" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="D40" s="20" t="s">
         <v>14</v>
@@ -2752,18 +2752,18 @@
         <v>20</v>
       </c>
       <c r="P40" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="Q40" s="9" t="s">
-        <v>236</v>
+        <v>244</v>
+      </c>
+      <c r="Q40" s="25" t="s">
+        <v>245</v>
       </c>
       <c r="R40" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="19" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
@@ -2784,267 +2784,105 @@
         <v>20</v>
       </c>
       <c r="P41" s="16" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Q41" s="15" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="R41" s="12" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A42" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="D42" s="17"/>
+      <c r="O42" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="P42" s="5" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="O42" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="P42" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="Q42" s="25" t="s">
-        <v>254</v>
-      </c>
-      <c r="R42" s="12" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A43" s="19" t="s">
-        <v>242</v>
-      </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="P43" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q43" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="R43" s="12" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="O44" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="P44" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q44" s="25" t="s">
-        <v>245</v>
-      </c>
-      <c r="R44" s="12" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" ht="72" x14ac:dyDescent="0.3">
-      <c r="A45" s="19" t="s">
-        <v>246</v>
-      </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="N45" s="18"/>
-      <c r="O45" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="P45" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="Q45" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="R45" s="12" t="s">
-        <v>264</v>
-      </c>
+      <c r="Q42" s="25"/>
+      <c r="R42" s="12"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P43" s="6"/>
+      <c r="Q43" s="20"/>
+      <c r="R43" s="7"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="P44" s="6"/>
+      <c r="Q44" s="20"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="P45" s="1"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="O46" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="P46" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="Q46" s="25" t="s">
-        <v>249</v>
-      </c>
-      <c r="R46" s="12" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="P47" s="16" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q47" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="R47" s="12" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="D48" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="O48" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="P48" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q48" s="25" t="s">
-        <v>258</v>
-      </c>
-      <c r="R48" s="12" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="P49" s="6"/>
-      <c r="Q49" s="20"/>
-      <c r="R49" s="7"/>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P46" s="1"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="P47" s="1"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="P48" s="1"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="P49" s="1"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
-      <c r="P50" s="6"/>
-      <c r="Q50" s="20"/>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="P51" s="1"/>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="P52" s="1"/>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="P53" s="1"/>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="P54" s="1"/>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="P55" s="1"/>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="P56" s="1"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="P50" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3074,28 +2912,21 @@
     <hyperlink ref="Q29" r:id="rId24" xr:uid="{918B8AC5-180E-4940-AB65-07EB923E4F5F}"/>
     <hyperlink ref="Q30" r:id="rId25" xr:uid="{5659E90E-47CC-402D-9CAA-E14C0FEBCE76}"/>
     <hyperlink ref="Q31" r:id="rId26" xr:uid="{68B94B25-7CC7-47EC-BD90-681D14787DDD}"/>
-    <hyperlink ref="Q33" r:id="rId27" xr:uid="{EC5E9B27-8100-49D6-AE4B-BEB7F2804023}"/>
-    <hyperlink ref="Q34" r:id="rId28" xr:uid="{194DDE3C-9541-4C9A-880B-258DBFC87759}"/>
-    <hyperlink ref="Q35" r:id="rId29" xr:uid="{28B0133F-CC3A-4748-845D-FE2FDAF2A56D}"/>
-    <hyperlink ref="Q17" r:id="rId30" xr:uid="{4B1D7DE7-B6CB-4F4B-AA12-9C58259214CD}"/>
-    <hyperlink ref="Q36" r:id="rId31" xr:uid="{03F67F50-AC64-4992-86C7-3FB6E7566854}"/>
-    <hyperlink ref="Q20" r:id="rId32" xr:uid="{E01F87EB-29CE-4362-A309-CCFCDFCB7018}"/>
-    <hyperlink ref="Q38" r:id="rId33" xr:uid="{F786FBAD-02D8-4EA9-988B-B28AA52340BF}"/>
-    <hyperlink ref="Q37" r:id="rId34" xr:uid="{2C40B6BD-3929-45C7-90C6-D357A3FD8533}"/>
-    <hyperlink ref="Q39" r:id="rId35" xr:uid="{8C97A54F-A448-48DD-BF59-94926D0EE56B}"/>
-    <hyperlink ref="Q40" r:id="rId36" display="https://github.com/ParadropLabs/Paradrop" xr:uid="{88850A09-8A0E-4EB7-9116-8E1E9016E581}"/>
-    <hyperlink ref="Q41" r:id="rId37" display="https://github.com/fogbed/fogbed" xr:uid="{2BF05C0E-CD23-4866-A523-020F58678AC1}"/>
-    <hyperlink ref="Q43" r:id="rId38" xr:uid="{9E691AAB-3716-4D4F-9A16-BE2946E764AB}"/>
-    <hyperlink ref="Q44" r:id="rId39" xr:uid="{901C773D-FD51-4A15-B831-B724F07F122D}"/>
-    <hyperlink ref="Q45" r:id="rId40" xr:uid="{9BD6403B-F868-4093-97D7-8C56FD11E6D1}"/>
-    <hyperlink ref="Q46" r:id="rId41" xr:uid="{3CF6F06A-BDD3-4EB1-93AA-47377A199191}"/>
-    <hyperlink ref="Q47" r:id="rId42" xr:uid="{0303BD42-06DC-4BA2-9CC6-753B105C924E}"/>
-    <hyperlink ref="Q42" r:id="rId43" xr:uid="{F439ED57-CDA7-480E-9ADE-AA2DAE8E24A0}"/>
-    <hyperlink ref="Q48" r:id="rId44" xr:uid="{914C127C-F393-458C-B313-98F473690CE0}"/>
-    <hyperlink ref="Q24" r:id="rId45" display="http://simgrid.gforge.inria.fr" xr:uid="{2B37E65A-5594-439A-AF61-442EC7378B73}"/>
+    <hyperlink ref="Q33" r:id="rId27" xr:uid="{28B0133F-CC3A-4748-845D-FE2FDAF2A56D}"/>
+    <hyperlink ref="Q17" r:id="rId28" xr:uid="{4B1D7DE7-B6CB-4F4B-AA12-9C58259214CD}"/>
+    <hyperlink ref="Q20" r:id="rId29" xr:uid="{E01F87EB-29CE-4362-A309-CCFCDFCB7018}"/>
+    <hyperlink ref="Q34" r:id="rId30" xr:uid="{F786FBAD-02D8-4EA9-988B-B28AA52340BF}"/>
+    <hyperlink ref="Q35" r:id="rId31" xr:uid="{8C97A54F-A448-48DD-BF59-94926D0EE56B}"/>
+    <hyperlink ref="Q36" r:id="rId32" display="https://github.com/ParadropLabs/Paradrop" xr:uid="{88850A09-8A0E-4EB7-9116-8E1E9016E581}"/>
+    <hyperlink ref="Q37" r:id="rId33" display="https://github.com/fogbed/fogbed" xr:uid="{2BF05C0E-CD23-4866-A523-020F58678AC1}"/>
+    <hyperlink ref="Q39" r:id="rId34" xr:uid="{9E691AAB-3716-4D4F-9A16-BE2946E764AB}"/>
+    <hyperlink ref="Q40" r:id="rId35" xr:uid="{901C773D-FD51-4A15-B831-B724F07F122D}"/>
+    <hyperlink ref="Q41" r:id="rId36" xr:uid="{0303BD42-06DC-4BA2-9CC6-753B105C924E}"/>
+    <hyperlink ref="Q38" r:id="rId37" xr:uid="{F439ED57-CDA7-480E-9ADE-AA2DAE8E24A0}"/>
+    <hyperlink ref="Q24" r:id="rId38" display="http://simgrid.gforge.inria.fr" xr:uid="{2B37E65A-5594-439A-AF61-442EC7378B73}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId46"/>
+  <pageSetup orientation="portrait" r:id="rId39"/>
 </worksheet>
 </file>
 
@@ -3103,8 +2934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0ECC1E-0276-4E25-9545-6E5C69A5CE5C}">
   <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J80" sqref="J80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3153,7 +2984,7 @@
         <v>196</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="N1" s="20" t="s">
         <v>195</v>
@@ -3206,7 +3037,7 @@
         <v>157</v>
       </c>
       <c r="R2" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3262,7 +3093,7 @@
         <v>157</v>
       </c>
       <c r="R3" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -3292,7 +3123,7 @@
         <v>157</v>
       </c>
       <c r="R4" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -3322,7 +3153,7 @@
         <v>157</v>
       </c>
       <c r="R5" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -3352,7 +3183,7 @@
         <v>157</v>
       </c>
       <c r="R6" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -3388,7 +3219,7 @@
         <v>157</v>
       </c>
       <c r="R7" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -3424,7 +3255,7 @@
         <v>157</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -3454,7 +3285,7 @@
         <v>157</v>
       </c>
       <c r="R9" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="72" x14ac:dyDescent="0.3">
@@ -3484,7 +3315,7 @@
         <v>157</v>
       </c>
       <c r="R10" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -3514,7 +3345,7 @@
         <v>157</v>
       </c>
       <c r="R11" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -3560,7 +3391,7 @@
         <v>157</v>
       </c>
       <c r="R12" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -3590,7 +3421,7 @@
         <v>157</v>
       </c>
       <c r="R13" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -3620,7 +3451,7 @@
         <v>157</v>
       </c>
       <c r="R14" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -3650,7 +3481,7 @@
         <v>157</v>
       </c>
       <c r="R15" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -3702,7 +3533,7 @@
         <v>157</v>
       </c>
       <c r="R16" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -3732,7 +3563,7 @@
         <v>155</v>
       </c>
       <c r="R17" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -3764,7 +3595,7 @@
         <v>209</v>
       </c>
       <c r="R18" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -3794,7 +3625,7 @@
         <v>212</v>
       </c>
       <c r="R19" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -3824,7 +3655,7 @@
         <v>150</v>
       </c>
       <c r="R20" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -3854,7 +3685,7 @@
         <v>147</v>
       </c>
       <c r="R21" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -3884,7 +3715,7 @@
         <v>144</v>
       </c>
       <c r="R22" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
@@ -3914,7 +3745,7 @@
         <v>141</v>
       </c>
       <c r="R23" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -3944,7 +3775,7 @@
         <v>226</v>
       </c>
       <c r="R24" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -3974,7 +3805,7 @@
         <v>137</v>
       </c>
       <c r="R25" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4004,7 +3835,7 @@
         <v>135</v>
       </c>
       <c r="R26" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4034,7 +3865,7 @@
         <v>132</v>
       </c>
       <c r="R27" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
@@ -4058,7 +3889,7 @@
       <c r="P28" s="16"/>
       <c r="Q28" s="18"/>
       <c r="R28" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4090,7 +3921,7 @@
         <v>128</v>
       </c>
       <c r="R29" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4128,7 +3959,7 @@
         <v>124</v>
       </c>
       <c r="R30" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4184,7 +4015,7 @@
         <v>118</v>
       </c>
       <c r="R31" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4240,7 +4071,7 @@
         <v>111</v>
       </c>
       <c r="R32" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -4288,7 +4119,7 @@
         <v>106</v>
       </c>
       <c r="R33" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -4328,7 +4159,7 @@
         <v>101</v>
       </c>
       <c r="R34" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4362,7 +4193,7 @@
       </c>
       <c r="Q35" s="20"/>
       <c r="R35" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4410,7 +4241,7 @@
         <v>95</v>
       </c>
       <c r="R36" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4444,7 +4275,7 @@
       <c r="P37" s="13"/>
       <c r="Q37" s="20"/>
       <c r="R37" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="72" x14ac:dyDescent="0.3">
@@ -4480,7 +4311,7 @@
       </c>
       <c r="Q38" s="15"/>
       <c r="R38" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4522,7 +4353,7 @@
       <c r="P39" s="13"/>
       <c r="Q39" s="20"/>
       <c r="R39" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
@@ -4572,7 +4403,7 @@
       </c>
       <c r="Q40" s="18"/>
       <c r="R40" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4620,7 +4451,7 @@
         <v>76</v>
       </c>
       <c r="R41" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4656,7 +4487,7 @@
       </c>
       <c r="Q42" s="18"/>
       <c r="R42" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4706,7 +4537,7 @@
         <v>66</v>
       </c>
       <c r="R43" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4742,7 +4573,7 @@
       </c>
       <c r="Q44" s="18"/>
       <c r="R44" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4776,7 +4607,7 @@
       </c>
       <c r="Q45" s="20"/>
       <c r="R45" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="72" x14ac:dyDescent="0.3">
@@ -4812,7 +4643,7 @@
         <v>57</v>
       </c>
       <c r="R46" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4848,7 +4679,7 @@
         <v>54</v>
       </c>
       <c r="R47" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
@@ -4884,7 +4715,7 @@
         <v>51</v>
       </c>
       <c r="R48" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4920,7 +4751,7 @@
         <v>46</v>
       </c>
       <c r="R49" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="50" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4956,7 +4787,7 @@
         <v>43</v>
       </c>
       <c r="R50" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="51" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -4992,7 +4823,7 @@
         <v>40</v>
       </c>
       <c r="R51" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.3">
@@ -5026,7 +4857,7 @@
       </c>
       <c r="Q52" s="18"/>
       <c r="R52" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="53" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -5060,7 +4891,7 @@
       </c>
       <c r="Q53" s="20"/>
       <c r="R53" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="54" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -5096,7 +4927,7 @@
         <v>31</v>
       </c>
       <c r="R54" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="55" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -5142,7 +4973,7 @@
       </c>
       <c r="Q55" s="20"/>
       <c r="R55" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="56" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -5184,7 +5015,7 @@
       <c r="P56" s="16"/>
       <c r="Q56" s="18"/>
       <c r="R56" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.3">
@@ -5214,7 +5045,7 @@
       <c r="P57" s="13"/>
       <c r="Q57" s="20"/>
       <c r="R57" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="58" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -5246,7 +5077,7 @@
         <v>12</v>
       </c>
       <c r="R58" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="59" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -5276,7 +5107,7 @@
         <v>9</v>
       </c>
       <c r="R59" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="60" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -5308,7 +5139,7 @@
         <v>6</v>
       </c>
       <c r="R60" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="61" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -5328,7 +5159,7 @@
         <v>223</v>
       </c>
       <c r="R61" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="62" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -5358,7 +5189,7 @@
         <v>229</v>
       </c>
       <c r="R62" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="63" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -5378,7 +5209,7 @@
         <v>228</v>
       </c>
       <c r="R63" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="64" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -5410,7 +5241,7 @@
         <v>232</v>
       </c>
       <c r="R64" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="65" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -5430,7 +5261,7 @@
         <v>236</v>
       </c>
       <c r="R65" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="66" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
@@ -5462,7 +5293,7 @@
         <v>239</v>
       </c>
       <c r="R66" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="67" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -5482,7 +5313,7 @@
         <v>254</v>
       </c>
       <c r="R67" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="68" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -5514,7 +5345,7 @@
         <v>240</v>
       </c>
       <c r="R68" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="69" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -5534,7 +5365,7 @@
         <v>245</v>
       </c>
       <c r="R69" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="70" spans="1:18" ht="72" x14ac:dyDescent="0.3">
@@ -5566,7 +5397,7 @@
         <v>248</v>
       </c>
       <c r="R70" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.3">
@@ -5586,7 +5417,7 @@
         <v>249</v>
       </c>
       <c r="R71" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="72" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
@@ -5618,12 +5449,12 @@
         <v>251</v>
       </c>
       <c r="R72" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="73" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D73" s="17" t="s">
         <v>14</v>
@@ -5632,13 +5463,13 @@
         <v>20</v>
       </c>
       <c r="P73" s="5" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="Q73" s="25" t="s">
         <v>258</v>
       </c>
       <c r="R73" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>